<commit_message>
update model resampling comparison
</commit_message>
<xml_diff>
--- a/Model_Resampling_Comparison.xlsx
+++ b/Model_Resampling_Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bk-covid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4BB9BC-969B-48E8-94B7-60C11BE075D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC2DFD3-8654-4C24-9446-4D6D77DA28C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55EEDD8E-35A0-466A-BF5D-2565983A03A7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="23">
   <si>
     <t>Target</t>
   </si>
@@ -90,6 +90,21 @@
   <si>
     <t>Mean
 (Resampling)</t>
+  </si>
+  <si>
+    <t>DL_FN</t>
+  </si>
+  <si>
+    <t>GBC_FN</t>
+  </si>
+  <si>
+    <t>EEC_FN</t>
+  </si>
+  <si>
+    <t>Old Data</t>
+  </si>
+  <si>
+    <t>New Data: including 'closed_contact', and 'another_complication'</t>
   </si>
 </sst>
 </file>
@@ -97,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -131,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +159,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -284,6 +305,187 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -293,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -319,13 +521,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -346,14 +548,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,6 +576,136 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -692,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F70DE5C-1191-4524-AC78-9781FB521876}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,7 +1038,8 @@
     <col min="6" max="7" width="15.33203125" style="1" customWidth="1"/>
     <col min="8" max="9" width="12.44140625" style="1" customWidth="1"/>
     <col min="10" max="11" width="11.6640625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="1"/>
     <col min="15" max="15" width="12.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -718,51 +1049,53 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="28" t="s">
+      <c r="I3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="28" t="s">
+      <c r="K3" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="29"/>
-      <c r="O3" s="30" t="s">
+      <c r="M3" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="27"/>
+      <c r="O3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="26" t="s">
         <v>15</v>
       </c>
       <c r="Q3" s="6"/>
@@ -788,10 +1121,10 @@
         <v>175</v>
       </c>
       <c r="H4" s="9">
-        <v>0.82923999999999998</v>
+        <v>0.84970999999999997</v>
       </c>
       <c r="I4" s="8">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="J4" s="9">
         <v>0.84918000000000005</v>
@@ -807,210 +1140,210 @@
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="11">
-        <f>AVERAGE(D4,F4,H4,J4,L4)</f>
-        <v>0.84486880000000009</v>
+        <f t="shared" ref="O4:P9" si="0">AVERAGE(D4,F4,H4,J4,L4)</f>
+        <v>0.84896280000000002</v>
       </c>
       <c r="P4" s="12">
-        <f>AVERAGE(E4,G4,I4,K4,M4)</f>
-        <v>137.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>131.4</v>
       </c>
       <c r="Q4" s="13"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="35">
         <v>0.83499699999999999</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="34">
         <v>185</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="35">
         <v>0.82452700000000001</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="34">
         <v>209</v>
       </c>
-      <c r="H5" s="9">
-        <v>0.64036000000000004</v>
-      </c>
-      <c r="I5" s="8">
-        <v>278</v>
-      </c>
-      <c r="J5" s="9">
-        <v>0.78612000000000004</v>
-      </c>
-      <c r="K5" s="8">
-        <v>284</v>
-      </c>
-      <c r="L5" s="9">
+      <c r="H5" s="35">
+        <v>0.77054</v>
+      </c>
+      <c r="I5" s="34">
+        <v>266</v>
+      </c>
+      <c r="J5" s="35">
+        <v>0.80337000000000003</v>
+      </c>
+      <c r="K5" s="34">
+        <v>254</v>
+      </c>
+      <c r="L5" s="35">
         <v>0.85529100000000002</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="34">
         <v>128</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11">
-        <f>AVERAGE(D5,F5,H5,J5,L5)</f>
-        <v>0.78825900000000004</v>
-      </c>
-      <c r="P5" s="14">
-        <f>AVERAGE(E5,G5,I5,K5,M5)</f>
-        <v>216.8</v>
-      </c>
-      <c r="Q5" s="13"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="37">
+        <f t="shared" si="0"/>
+        <v>0.81774500000000006</v>
+      </c>
+      <c r="P5" s="38">
+        <f t="shared" si="0"/>
+        <v>208.4</v>
+      </c>
+      <c r="Q5" s="67"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="47">
         <v>0.87381600000000004</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="46">
         <v>14</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="47">
         <v>0.87388299999999997</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="46">
         <v>14</v>
       </c>
-      <c r="H6" s="9">
-        <v>0.69696999999999998</v>
-      </c>
-      <c r="I6" s="8">
-        <v>40</v>
-      </c>
-      <c r="J6" s="9">
+      <c r="H6" s="47">
+        <v>0.78707000000000005</v>
+      </c>
+      <c r="I6" s="46">
+        <v>39</v>
+      </c>
+      <c r="J6" s="47">
         <v>0.80215999999999998</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="46">
         <v>37</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="47">
         <v>0.87103299999999995</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="46">
         <v>14</v>
       </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="11">
-        <f>AVERAGE(D6,F6,H6,J6,L6)</f>
-        <v>0.82357239999999998</v>
-      </c>
-      <c r="P6" s="12">
-        <f>AVERAGE(E6,G6,I6,K6,M6)</f>
-        <v>23.8</v>
-      </c>
-      <c r="Q6" s="13"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N6" s="48"/>
+      <c r="O6" s="49">
+        <f t="shared" si="0"/>
+        <v>0.84159239999999991</v>
+      </c>
+      <c r="P6" s="69">
+        <f t="shared" si="0"/>
+        <v>23.6</v>
+      </c>
+      <c r="Q6" s="70"/>
+    </row>
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="53">
         <v>0.82785500000000001</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="52">
         <v>29</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="53">
         <v>0.87388299999999997</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="52">
         <v>14</v>
       </c>
-      <c r="H7" s="9">
-        <v>0.32574999999999998</v>
-      </c>
-      <c r="I7" s="8">
-        <v>89</v>
-      </c>
-      <c r="J7" s="9">
+      <c r="H7" s="53">
+        <v>0.64031000000000005</v>
+      </c>
+      <c r="I7" s="52">
+        <v>86</v>
+      </c>
+      <c r="J7" s="53">
         <v>0.51844999999999997</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="52">
         <v>126</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="53">
         <v>0.87103299999999995</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="52">
         <v>14</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="11">
-        <f>AVERAGE(D7,F7,H7,J7,L7)</f>
-        <v>0.68339420000000006</v>
-      </c>
-      <c r="P7" s="14">
-        <f>AVERAGE(E7,G7,I7,K7,M7)</f>
-        <v>54.4</v>
-      </c>
-      <c r="Q7" s="13"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="55">
+        <f t="shared" si="0"/>
+        <v>0.74630620000000003</v>
+      </c>
+      <c r="P7" s="71">
+        <f t="shared" si="0"/>
+        <v>53.8</v>
+      </c>
+      <c r="Q7" s="72"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="41">
         <v>0.839314</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="40">
         <v>45</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="41">
         <v>0.84023700000000001</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="40">
         <v>46</v>
       </c>
-      <c r="H8" s="9">
-        <v>0.69386999999999999</v>
-      </c>
-      <c r="I8" s="8">
-        <v>75</v>
-      </c>
-      <c r="J8" s="9">
+      <c r="H8" s="41">
+        <v>0.78952999999999995</v>
+      </c>
+      <c r="I8" s="40">
+        <v>67</v>
+      </c>
+      <c r="J8" s="41">
         <v>0.80788000000000004</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="40">
         <v>63</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="41">
         <v>0.83376899999999998</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="40">
         <v>49</v>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="11">
-        <f>AVERAGE(D8,F8,H8,J8,L8)</f>
-        <v>0.80301399999999989</v>
-      </c>
-      <c r="P8" s="12">
-        <f>AVERAGE(E8,G8,I8,K8,M8)</f>
-        <v>55.6</v>
-      </c>
-      <c r="Q8" s="13"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="43">
+        <f t="shared" si="0"/>
+        <v>0.82214600000000004</v>
+      </c>
+      <c r="P8" s="44">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="Q8" s="68"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
@@ -1033,10 +1366,10 @@
         <v>46</v>
       </c>
       <c r="H9" s="9">
-        <v>0.34286</v>
+        <v>0.65549000000000002</v>
       </c>
       <c r="I9" s="8">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="J9" s="9">
         <v>0.58259000000000005</v>
@@ -1052,12 +1385,12 @@
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="11">
-        <f>AVERAGE(D9,F9,H9,J9,L9)</f>
-        <v>0.67166619999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.73419220000000007</v>
       </c>
       <c r="P9" s="14">
-        <f>AVERAGE(E9,G9,I9,K9,M9)</f>
-        <v>108.8</v>
+        <f t="shared" si="0"/>
+        <v>105.2</v>
       </c>
       <c r="Q9" s="13"/>
     </row>
@@ -1087,43 +1420,43 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9">
-        <f>AVERAGE(D4:D9)</f>
+        <f t="shared" ref="D11:M11" si="1">AVERAGE(D4:D9)</f>
         <v>0.83234233333333341</v>
       </c>
       <c r="E11" s="17">
-        <f>AVERAGE(E4:E9)</f>
+        <f t="shared" si="1"/>
         <v>80.666666666666671</v>
       </c>
       <c r="F11" s="18">
-        <f>AVERAGE(F4:F9)</f>
+        <f t="shared" si="1"/>
         <v>0.84736716666666656</v>
       </c>
       <c r="G11" s="19">
-        <f>AVERAGE(G4:G9)</f>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="H11" s="9">
-        <f>AVERAGE(H4:H9)</f>
-        <v>0.588175</v>
+        <f t="shared" si="1"/>
+        <v>0.74877500000000008</v>
       </c>
       <c r="I11" s="17">
-        <f>AVERAGE(I4:I9)</f>
-        <v>129.16666666666666</v>
+        <f t="shared" si="1"/>
+        <v>116.83333333333333</v>
       </c>
       <c r="J11" s="9">
-        <f>AVERAGE(J4:J9)</f>
-        <v>0.72439666666666669</v>
+        <f t="shared" si="1"/>
+        <v>0.72727166666666676</v>
       </c>
       <c r="K11" s="17">
-        <f>AVERAGE(K4:K9)</f>
-        <v>140.16666666666666</v>
+        <f t="shared" si="1"/>
+        <v>135.16666666666666</v>
       </c>
       <c r="L11" s="18">
-        <f>AVERAGE(L4:L9)</f>
+        <f t="shared" si="1"/>
         <v>0.85336433333333339</v>
       </c>
       <c r="M11" s="19">
-        <f>AVERAGE(M4:M9)</f>
+        <f t="shared" si="1"/>
         <v>63.666666666666664</v>
       </c>
       <c r="N11" s="10"/>
@@ -1131,96 +1464,475 @@
       <c r="P11" s="10"/>
       <c r="Q11" s="13"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="13"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="21"/>
+    <row r="12" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="24"/>
+    </row>
+    <row r="13" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="21"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="21"/>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="27"/>
+      <c r="O15" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="26"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="63">
+        <v>0.86495</v>
+      </c>
+      <c r="E16" s="64">
+        <v>101</v>
+      </c>
+      <c r="F16" s="63">
+        <v>0.86567000000000005</v>
+      </c>
+      <c r="G16" s="64">
+        <v>103</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.83172000000000001</v>
+      </c>
+      <c r="I16" s="8">
+        <v>139</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.84550999999999998</v>
+      </c>
+      <c r="K16" s="8">
+        <v>140</v>
+      </c>
+      <c r="L16" s="63">
+        <v>0.86316000000000004</v>
+      </c>
+      <c r="M16" s="64">
+        <v>113</v>
+      </c>
+      <c r="N16" s="10"/>
+      <c r="O16" s="11">
+        <f t="shared" ref="O16:O21" si="2">AVERAGE(D16,F16,H16,J16,L16)</f>
+        <v>0.85420199999999991</v>
+      </c>
+      <c r="P16" s="12">
+        <f t="shared" ref="P16:P21" si="3">AVERAGE(E16,G16,I16,K16,M16)</f>
+        <v>119.2</v>
+      </c>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4"/>
+      <c r="B17" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="35">
+        <v>0.83245999999999998</v>
+      </c>
+      <c r="E17" s="34">
+        <v>191</v>
+      </c>
+      <c r="F17" s="35">
+        <v>0.82216</v>
+      </c>
+      <c r="G17" s="34">
+        <v>211</v>
+      </c>
+      <c r="H17" s="35">
+        <v>0.65190999999999999</v>
+      </c>
+      <c r="I17" s="34">
+        <v>402</v>
+      </c>
+      <c r="J17" s="61">
+        <v>0.80562999999999996</v>
+      </c>
+      <c r="K17" s="62">
+        <v>244</v>
+      </c>
+      <c r="L17" s="61">
+        <v>0.86316000000000004</v>
+      </c>
+      <c r="M17" s="62">
+        <v>113</v>
+      </c>
+      <c r="N17" s="36"/>
+      <c r="O17" s="37">
+        <f t="shared" si="2"/>
+        <v>0.79506399999999999</v>
+      </c>
+      <c r="P17" s="38">
+        <f t="shared" si="3"/>
+        <v>232.2</v>
+      </c>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="59">
+        <v>0.88092999999999999</v>
+      </c>
+      <c r="E18" s="60">
+        <v>11</v>
+      </c>
+      <c r="F18" s="59">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="G18" s="60">
+        <v>11</v>
+      </c>
+      <c r="H18" s="47">
+        <v>0.77793000000000001</v>
+      </c>
+      <c r="I18" s="46">
+        <v>42</v>
+      </c>
+      <c r="J18" s="59">
+        <v>0.83631</v>
+      </c>
+      <c r="K18" s="60">
+        <v>26</v>
+      </c>
+      <c r="L18" s="59">
+        <v>0.87980999999999998</v>
+      </c>
+      <c r="M18" s="60">
+        <v>10</v>
+      </c>
+      <c r="N18" s="48"/>
+      <c r="O18" s="49">
+        <f t="shared" si="2"/>
+        <v>0.85119600000000006</v>
+      </c>
+      <c r="P18" s="50">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="Q18" s="32"/>
+    </row>
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="57">
+        <v>0.88058999999999998</v>
+      </c>
+      <c r="E19" s="58">
+        <v>11</v>
+      </c>
+      <c r="F19" s="57">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="G19" s="58">
+        <v>11</v>
+      </c>
+      <c r="H19" s="57">
+        <v>0.64105000000000001</v>
+      </c>
+      <c r="I19" s="58">
+        <v>83</v>
+      </c>
+      <c r="J19" s="57">
+        <v>0.57225999999999999</v>
+      </c>
+      <c r="K19" s="58">
+        <v>107</v>
+      </c>
+      <c r="L19" s="57">
+        <v>0.87980999999999998</v>
+      </c>
+      <c r="M19" s="58">
+        <v>10</v>
+      </c>
+      <c r="N19" s="54"/>
+      <c r="O19" s="55">
+        <f t="shared" si="2"/>
+        <v>0.77094200000000002</v>
+      </c>
+      <c r="P19" s="56">
+        <f t="shared" si="3"/>
+        <v>44.4</v>
+      </c>
+      <c r="Q19" s="32"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="41">
+        <v>0.83609999999999995</v>
+      </c>
+      <c r="E20" s="40">
+        <v>49</v>
+      </c>
+      <c r="F20" s="41">
+        <v>0.83153999999999995</v>
+      </c>
+      <c r="G20" s="40">
+        <v>50</v>
+      </c>
+      <c r="H20" s="41">
+        <v>0.77414000000000005</v>
+      </c>
+      <c r="I20" s="40">
+        <v>82</v>
+      </c>
+      <c r="J20" s="41">
+        <v>0.80110000000000003</v>
+      </c>
+      <c r="K20" s="40">
+        <v>70</v>
+      </c>
+      <c r="L20" s="65">
+        <v>0.83762000000000003</v>
+      </c>
+      <c r="M20" s="66">
+        <v>48</v>
+      </c>
+      <c r="N20" s="42"/>
+      <c r="O20" s="43">
+        <f t="shared" si="2"/>
+        <v>0.81609999999999994</v>
+      </c>
+      <c r="P20" s="44">
+        <f t="shared" si="3"/>
+        <v>59.8</v>
+      </c>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="63">
+        <v>0.82008999999999999</v>
+      </c>
+      <c r="E21" s="64">
+        <v>59</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.83140000000000003</v>
+      </c>
+      <c r="G21" s="8">
+        <v>50</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.61629</v>
+      </c>
+      <c r="I21" s="8">
+        <v>171</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.54967999999999995</v>
+      </c>
+      <c r="K21" s="8">
+        <v>220</v>
+      </c>
+      <c r="L21" s="63">
+        <v>0.83762000000000003</v>
+      </c>
+      <c r="M21" s="64">
+        <v>48</v>
+      </c>
+      <c r="N21" s="10"/>
+      <c r="O21" s="11">
+        <f t="shared" si="2"/>
+        <v>0.731016</v>
+      </c>
+      <c r="P21" s="14">
+        <f t="shared" si="3"/>
+        <v>109.6</v>
+      </c>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="13"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9">
+        <f t="shared" ref="D23:M23" si="4">AVERAGE(D16:D21)</f>
+        <v>0.85251999999999983</v>
+      </c>
+      <c r="E23" s="17">
+        <f t="shared" si="4"/>
+        <v>70.333333333333329</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" si="4"/>
+        <v>0.85212833333333349</v>
+      </c>
+      <c r="G23" s="19">
+        <f t="shared" si="4"/>
+        <v>72.666666666666671</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" si="4"/>
+        <v>0.71550666666666674</v>
+      </c>
+      <c r="I23" s="17">
+        <f t="shared" si="4"/>
+        <v>153.16666666666666</v>
+      </c>
+      <c r="J23" s="9">
+        <f t="shared" si="4"/>
+        <v>0.73508166666666652</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="4"/>
+        <v>134.5</v>
+      </c>
+      <c r="L23" s="18">
+        <f t="shared" si="4"/>
+        <v>0.86019666666666683</v>
+      </c>
+      <c r="M23" s="19">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="N23" s="10"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>